<commit_message>
Add import for Martial
</commit_message>
<xml_diff>
--- a/src/assets/template/2-Mau-Chuan_Thi_Quyen.xlsx
+++ b/src/assets/template/2-Mau-Chuan_Thi_Quyen.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Project\cocvuong-react\src\assets\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Project\cocvuong.com\src\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE0CC35-D2AE-4FF3-9186-9213D3757E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F93002-8C13-49E7-85E3-B78F97D15822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30950" yWindow="-320" windowWidth="21600" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="14" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">data!$A$1:$C$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">data!$A$1:$D$48</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="73">
   <si>
     <t>Hoàng Minh Tiến</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>SE171951</t>
+  </si>
+  <si>
+    <t>QUỐC GIA</t>
+  </si>
+  <si>
+    <t>VN</t>
   </si>
 </sst>
 </file>
@@ -341,7 +347,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,25 +636,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB2DDB7-F224-4251-AE4D-22EB2212EF5D}">
-  <dimension ref="A1:C161"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -658,8 +666,11 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -669,8 +680,11 @@
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -680,8 +694,11 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -691,8 +708,11 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -702,8 +722,11 @@
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -713,8 +736,11 @@
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -724,8 +750,11 @@
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -735,22 +764,27 @@
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -760,8 +794,11 @@
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -771,8 +808,11 @@
       <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2</v>
       </c>
@@ -782,8 +822,11 @@
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -793,8 +836,11 @@
       <c r="C15" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -804,8 +850,11 @@
       <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>5</v>
       </c>
@@ -815,8 +864,11 @@
       <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>6</v>
       </c>
@@ -826,8 +878,11 @@
       <c r="C18" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>7</v>
       </c>
@@ -837,8 +892,11 @@
       <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>8</v>
       </c>
@@ -848,8 +906,11 @@
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>9</v>
       </c>
@@ -859,22 +920,27 @@
       <c r="C21" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -884,8 +950,11 @@
       <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -895,8 +964,11 @@
       <c r="C25" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>34</v>
@@ -904,8 +976,11 @@
       <c r="C26" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>35</v>
@@ -913,8 +988,11 @@
       <c r="C27" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>2</v>
       </c>
@@ -924,8 +1002,11 @@
       <c r="C28" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>37</v>
@@ -933,8 +1014,11 @@
       <c r="C29" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>39</v>
@@ -942,8 +1026,11 @@
       <c r="C30" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>3</v>
       </c>
@@ -953,8 +1040,11 @@
       <c r="C31" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>43</v>
@@ -962,8 +1052,11 @@
       <c r="C32" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
         <v>45</v>
@@ -971,22 +1064,27 @@
       <c r="C33" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -996,8 +1094,11 @@
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1</v>
       </c>
@@ -1007,8 +1108,11 @@
       <c r="C37" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
         <v>50</v>
@@ -1016,8 +1120,11 @@
       <c r="C38" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D38" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
         <v>52</v>
@@ -1025,8 +1132,11 @@
       <c r="C39" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
         <v>54</v>
@@ -1034,8 +1144,11 @@
       <c r="C40" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>2</v>
       </c>
@@ -1045,8 +1158,11 @@
       <c r="C41" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
         <v>57</v>
@@ -1054,8 +1170,11 @@
       <c r="C42" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
         <v>59</v>
@@ -1063,8 +1182,11 @@
       <c r="C43" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
         <v>61</v>
@@ -1072,8 +1194,11 @@
       <c r="C44" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D44" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>3</v>
       </c>
@@ -1083,8 +1208,11 @@
       <c r="C45" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
         <v>65</v>
@@ -1092,8 +1220,11 @@
       <c r="C46" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
         <v>67</v>
@@ -1101,14 +1232,20 @@
       <c r="C47" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>70</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>